<commit_message>
Lista chequeo de codificacion
</commit_message>
<xml_diff>
--- a/documentos/Formatos de calidad/Formato de lista  de chequeo codificación.xlsx
+++ b/documentos/Formatos de calidad/Formato de lista  de chequeo codificación.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dasaca\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\laravel\produccionmarroquineria\documentos\Formatos de calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Datos Generales</t>
   </si>
@@ -131,6 +131,18 @@
     <t>FORMATO DE CHEQUEO 
 PARA REVISIÓN DE CÓDIGO</t>
   </si>
+  <si>
+    <t>Oven Dario Lame Gomez</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>En las pruebas realizadas, se encuentran algunos problemas de codificacion, en cuanto a funcionalidad del sistema.</t>
+  </si>
+  <si>
+    <t>Planificacion  de la produccion para la linea tecnologica de vestuario inteligente CDTI</t>
+  </si>
 </sst>
 </file>
 
@@ -815,6 +827,33 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -824,14 +863,209 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -878,18 +1112,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -928,216 +1150,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1157,7 +1169,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1177,7 +1189,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1189,7 +1201,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1209,7 +1221,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1225,7 +1237,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1241,7 +1253,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1265,7 +1277,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1281,7 +1293,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3687,8 +3699,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="B1:AD25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:W5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3709,124 +3721,124 @@
   <sheetData>
     <row r="1" spans="2:30" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="91"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="69" t="s">
+      <c r="B2" s="93"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="61"/>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="62"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="66"/>
     </row>
     <row r="3" spans="2:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="94"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="74"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="65"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="77"/>
+      <c r="T3" s="77"/>
+      <c r="U3" s="77"/>
+      <c r="V3" s="77"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="67"/>
+      <c r="Y3" s="68"/>
+      <c r="Z3" s="68"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="69"/>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="94"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="85" t="s">
+      <c r="B4" s="96"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="63"/>
-      <c r="Y4" s="64"/>
-      <c r="Z4" s="64"/>
-      <c r="AA4" s="64"/>
-      <c r="AB4" s="65"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="89"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="68"/>
+      <c r="Z4" s="68"/>
+      <c r="AA4" s="68"/>
+      <c r="AB4" s="69"/>
     </row>
     <row r="5" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="97"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="89"/>
-      <c r="T5" s="89"/>
-      <c r="U5" s="89"/>
-      <c r="V5" s="89"/>
-      <c r="W5" s="90"/>
-      <c r="X5" s="66"/>
-      <c r="Y5" s="67"/>
-      <c r="Z5" s="67"/>
-      <c r="AA5" s="67"/>
-      <c r="AB5" s="68"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="91"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
+      <c r="W5" s="92"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="71"/>
+      <c r="Z5" s="71"/>
+      <c r="AA5" s="71"/>
+      <c r="AB5" s="72"/>
     </row>
     <row r="6" spans="2:30" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
@@ -3859,21 +3871,27 @@
     </row>
     <row r="7" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
-      <c r="C7" s="78" t="s">
+      <c r="C7" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="84"/>
-      <c r="O7" s="83"/>
+      <c r="I7" s="44">
+        <v>5</v>
+      </c>
+      <c r="J7" s="86"/>
+      <c r="K7" s="44">
+        <v>8</v>
+      </c>
+      <c r="L7" s="86"/>
+      <c r="M7" s="44">
+        <v>2016</v>
+      </c>
+      <c r="N7" s="45"/>
+      <c r="O7" s="86"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
@@ -3881,9 +3899,9 @@
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="14"/>
-      <c r="W7" s="79"/>
-      <c r="X7" s="80"/>
-      <c r="Y7" s="81"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="84"/>
+      <c r="Y7" s="85"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="4"/>
@@ -3918,565 +3936,620 @@
       <c r="AB8" s="4"/>
     </row>
     <row r="9" spans="2:30" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="76"/>
-      <c r="S9" s="76"/>
-      <c r="T9" s="76"/>
-      <c r="U9" s="76"/>
-      <c r="V9" s="76"/>
-      <c r="W9" s="76"/>
-      <c r="X9" s="76"/>
-      <c r="Y9" s="76"/>
-      <c r="Z9" s="76"/>
-      <c r="AA9" s="76"/>
-      <c r="AB9" s="77"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="80"/>
+      <c r="S9" s="80"/>
+      <c r="T9" s="80"/>
+      <c r="U9" s="80"/>
+      <c r="V9" s="80"/>
+      <c r="W9" s="80"/>
+      <c r="X9" s="80"/>
+      <c r="Y9" s="80"/>
+      <c r="Z9" s="80"/>
+      <c r="AA9" s="80"/>
+      <c r="AB9" s="81"/>
     </row>
     <row r="10" spans="2:30" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B10" s="116" t="s">
+      <c r="B10" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="117"/>
-      <c r="D10" s="117"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="121"/>
-      <c r="H10" s="121"/>
-      <c r="I10" s="121"/>
-      <c r="J10" s="121"/>
-      <c r="K10" s="121"/>
-      <c r="L10" s="121"/>
-      <c r="M10" s="121"/>
-      <c r="N10" s="121"/>
-      <c r="O10" s="121"/>
-      <c r="P10" s="121"/>
-      <c r="Q10" s="121"/>
-      <c r="R10" s="121"/>
-      <c r="S10" s="121"/>
-      <c r="T10" s="121"/>
-      <c r="U10" s="121"/>
-      <c r="V10" s="121"/>
-      <c r="W10" s="121"/>
-      <c r="X10" s="121"/>
-      <c r="Y10" s="121"/>
-      <c r="Z10" s="121"/>
-      <c r="AA10" s="121"/>
-      <c r="AB10" s="122"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="39"/>
+      <c r="S10" s="39"/>
+      <c r="T10" s="39"/>
+      <c r="U10" s="39"/>
+      <c r="V10" s="39"/>
+      <c r="W10" s="39"/>
+      <c r="X10" s="39"/>
+      <c r="Y10" s="39"/>
+      <c r="Z10" s="39"/>
+      <c r="AA10" s="39"/>
+      <c r="AB10" s="40"/>
     </row>
     <row r="11" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="115"/>
-      <c r="H11" s="115"/>
-      <c r="I11" s="115"/>
-      <c r="J11" s="115"/>
-      <c r="K11" s="115"/>
-      <c r="L11" s="115"/>
-      <c r="M11" s="115"/>
-      <c r="N11" s="115"/>
-      <c r="O11" s="115"/>
-      <c r="P11" s="115"/>
-      <c r="Q11" s="115"/>
-      <c r="R11" s="115"/>
-      <c r="S11" s="115"/>
-      <c r="T11" s="115"/>
-      <c r="U11" s="115" t="s">
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="V11" s="115"/>
-      <c r="W11" s="115"/>
-      <c r="X11" s="115"/>
-      <c r="Y11" s="115"/>
-      <c r="Z11" s="82"/>
-      <c r="AA11" s="84"/>
-      <c r="AB11" s="126"/>
+      <c r="V11" s="47"/>
+      <c r="W11" s="47"/>
+      <c r="X11" s="47"/>
+      <c r="Y11" s="47"/>
+      <c r="Z11" s="44">
+        <v>8</v>
+      </c>
+      <c r="AA11" s="45"/>
+      <c r="AB11" s="46"/>
     </row>
     <row r="12" spans="2:30" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="124"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="124"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="124"/>
-      <c r="L12" s="124"/>
-      <c r="M12" s="124"/>
-      <c r="N12" s="124"/>
-      <c r="O12" s="124"/>
-      <c r="P12" s="124"/>
-      <c r="Q12" s="124"/>
-      <c r="R12" s="124"/>
-      <c r="S12" s="124"/>
-      <c r="T12" s="124"/>
-      <c r="U12" s="124"/>
-      <c r="V12" s="124"/>
-      <c r="W12" s="124"/>
-      <c r="X12" s="124"/>
-      <c r="Y12" s="124"/>
-      <c r="Z12" s="124"/>
-      <c r="AA12" s="124"/>
-      <c r="AB12" s="125"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="42"/>
+      <c r="V12" s="42"/>
+      <c r="W12" s="42"/>
+      <c r="X12" s="42"/>
+      <c r="Y12" s="42"/>
+      <c r="Z12" s="42"/>
+      <c r="AA12" s="42"/>
+      <c r="AB12" s="43"/>
     </row>
     <row r="13" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36"/>
-      <c r="U13" s="36"/>
-      <c r="V13" s="36"/>
-      <c r="W13" s="36"/>
-      <c r="X13" s="36"/>
-      <c r="Y13" s="36"/>
-      <c r="Z13" s="36"/>
-      <c r="AA13" s="36"/>
-      <c r="AB13" s="37"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="110"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="110"/>
+      <c r="N13" s="110"/>
+      <c r="O13" s="110"/>
+      <c r="P13" s="110"/>
+      <c r="Q13" s="110"/>
+      <c r="R13" s="110"/>
+      <c r="S13" s="110"/>
+      <c r="T13" s="110"/>
+      <c r="U13" s="110"/>
+      <c r="V13" s="110"/>
+      <c r="W13" s="110"/>
+      <c r="X13" s="110"/>
+      <c r="Y13" s="110"/>
+      <c r="Z13" s="110"/>
+      <c r="AA13" s="110"/>
+      <c r="AB13" s="111"/>
     </row>
     <row r="14" spans="2:30" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32" t="s">
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="33"/>
-      <c r="S14" s="33"/>
-      <c r="T14" s="33"/>
-      <c r="U14" s="33"/>
-      <c r="V14" s="33"/>
-      <c r="W14" s="33"/>
-      <c r="X14" s="33"/>
-      <c r="Y14" s="33"/>
-      <c r="Z14" s="33"/>
-      <c r="AA14" s="33"/>
-      <c r="AB14" s="34"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="107"/>
+      <c r="J14" s="107"/>
+      <c r="K14" s="107"/>
+      <c r="L14" s="107"/>
+      <c r="M14" s="107"/>
+      <c r="N14" s="107"/>
+      <c r="O14" s="107"/>
+      <c r="P14" s="107"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="107"/>
+      <c r="S14" s="107"/>
+      <c r="T14" s="107"/>
+      <c r="U14" s="107"/>
+      <c r="V14" s="107"/>
+      <c r="W14" s="107"/>
+      <c r="X14" s="107"/>
+      <c r="Y14" s="107"/>
+      <c r="Z14" s="107"/>
+      <c r="AA14" s="107"/>
+      <c r="AB14" s="108"/>
       <c r="AD14" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:30" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40" t="s">
+      <c r="C15" s="113"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="41"/>
-      <c r="S15" s="41"/>
-      <c r="T15" s="41"/>
-      <c r="U15" s="41"/>
-      <c r="V15" s="41"/>
-      <c r="W15" s="41"/>
-      <c r="X15" s="41"/>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="41"/>
-      <c r="AA15" s="41"/>
-      <c r="AB15" s="42"/>
+      <c r="F15" s="115"/>
+      <c r="G15" s="115"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="115"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="115"/>
+      <c r="L15" s="115"/>
+      <c r="M15" s="115"/>
+      <c r="N15" s="115"/>
+      <c r="O15" s="115"/>
+      <c r="P15" s="115"/>
+      <c r="Q15" s="115"/>
+      <c r="R15" s="115"/>
+      <c r="S15" s="115"/>
+      <c r="T15" s="115"/>
+      <c r="U15" s="115"/>
+      <c r="V15" s="115"/>
+      <c r="W15" s="115"/>
+      <c r="X15" s="115"/>
+      <c r="Y15" s="115"/>
+      <c r="Z15" s="115"/>
+      <c r="AA15" s="115"/>
+      <c r="AB15" s="116"/>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="54" t="s">
+      <c r="C16" s="119"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
-      <c r="R16" s="57"/>
-      <c r="S16" s="57"/>
-      <c r="T16" s="57"/>
-      <c r="U16" s="58"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="57"/>
-      <c r="X16" s="57"/>
-      <c r="Y16" s="57"/>
-      <c r="Z16" s="57"/>
-      <c r="AA16" s="57"/>
-      <c r="AB16" s="59"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="119"/>
+      <c r="H16" s="119"/>
+      <c r="I16" s="119"/>
+      <c r="J16" s="119"/>
+      <c r="K16" s="119"/>
+      <c r="L16" s="119"/>
+      <c r="M16" s="119"/>
+      <c r="N16" s="120"/>
+      <c r="O16" s="126"/>
+      <c r="P16" s="127"/>
+      <c r="Q16" s="127"/>
+      <c r="R16" s="127"/>
+      <c r="S16" s="127"/>
+      <c r="T16" s="127"/>
+      <c r="U16" s="128"/>
+      <c r="V16" s="126"/>
+      <c r="W16" s="127"/>
+      <c r="X16" s="127"/>
+      <c r="Y16" s="127"/>
+      <c r="Z16" s="127"/>
+      <c r="AA16" s="127"/>
+      <c r="AB16" s="129"/>
     </row>
     <row r="17" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="51"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="53"/>
+      <c r="B17" s="121"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="125"/>
+      <c r="F17" s="122"/>
+      <c r="G17" s="122"/>
+      <c r="H17" s="122"/>
+      <c r="I17" s="122"/>
+      <c r="J17" s="122"/>
+      <c r="K17" s="122"/>
+      <c r="L17" s="122"/>
+      <c r="M17" s="122"/>
+      <c r="N17" s="123"/>
       <c r="O17" s="15" t="s">
         <v>7</v>
       </c>
       <c r="P17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="Q17" s="45" t="s">
+      <c r="Q17" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="R17" s="46"/>
-      <c r="S17" s="46"/>
-      <c r="T17" s="46"/>
-      <c r="U17" s="114"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+      <c r="U17" s="50"/>
       <c r="V17" s="17"/>
       <c r="W17" s="10"/>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="46"/>
-      <c r="Z17" s="46"/>
-      <c r="AA17" s="46"/>
-      <c r="AB17" s="47"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="49"/>
+      <c r="AA17" s="49"/>
+      <c r="AB17" s="117"/>
     </row>
     <row r="18" spans="2:28" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="27"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="30"/>
       <c r="O18" s="16"/>
       <c r="P18" s="9"/>
-      <c r="Q18" s="100"/>
-      <c r="R18" s="101"/>
-      <c r="S18" s="101"/>
-      <c r="T18" s="101"/>
-      <c r="U18" s="102"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="26"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="27"/>
       <c r="V18" s="18"/>
       <c r="W18" s="9"/>
-      <c r="X18" s="43"/>
-      <c r="Y18" s="43"/>
-      <c r="Z18" s="43"/>
-      <c r="AA18" s="43"/>
-      <c r="AB18" s="44"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="51"/>
+      <c r="AA18" s="51"/>
+      <c r="AB18" s="52"/>
     </row>
     <row r="19" spans="2:28" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25" t="s">
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="27"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="30"/>
       <c r="O19" s="16"/>
       <c r="P19" s="9"/>
-      <c r="Q19" s="100"/>
-      <c r="R19" s="101"/>
-      <c r="S19" s="101"/>
-      <c r="T19" s="101"/>
-      <c r="U19" s="102"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="27"/>
       <c r="V19" s="18"/>
       <c r="W19" s="9"/>
-      <c r="X19" s="43"/>
-      <c r="Y19" s="43"/>
-      <c r="Z19" s="43"/>
-      <c r="AA19" s="43"/>
-      <c r="AB19" s="44"/>
+      <c r="X19" s="51"/>
+      <c r="Y19" s="51"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="51"/>
+      <c r="AB19" s="52"/>
     </row>
     <row r="20" spans="2:28" s="8" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25" t="s">
+      <c r="C20" s="32"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="27"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="30"/>
       <c r="O20" s="16"/>
       <c r="P20" s="9"/>
-      <c r="Q20" s="100"/>
-      <c r="R20" s="101"/>
-      <c r="S20" s="101"/>
-      <c r="T20" s="101"/>
-      <c r="U20" s="102"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="27"/>
       <c r="V20" s="18"/>
       <c r="W20" s="9"/>
-      <c r="X20" s="127"/>
-      <c r="Y20" s="128"/>
-      <c r="Z20" s="128"/>
-      <c r="AA20" s="128"/>
-      <c r="AB20" s="129"/>
+      <c r="X20" s="22"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="24"/>
     </row>
     <row r="21" spans="2:28" s="8" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25" t="s">
+      <c r="C21" s="32"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="27"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="30"/>
       <c r="O21" s="16"/>
       <c r="P21" s="9"/>
-      <c r="Q21" s="100"/>
-      <c r="R21" s="101"/>
-      <c r="S21" s="101"/>
-      <c r="T21" s="101"/>
-      <c r="U21" s="102"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="27"/>
       <c r="V21" s="18"/>
       <c r="W21" s="9"/>
-      <c r="X21" s="43"/>
-      <c r="Y21" s="43"/>
-      <c r="Z21" s="43"/>
-      <c r="AA21" s="43"/>
-      <c r="AB21" s="44"/>
+      <c r="X21" s="51"/>
+      <c r="Y21" s="51"/>
+      <c r="Z21" s="51"/>
+      <c r="AA21" s="51"/>
+      <c r="AB21" s="52"/>
     </row>
     <row r="22" spans="2:28" s="8" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="25" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="27"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="30"/>
       <c r="O22" s="16"/>
       <c r="P22" s="9"/>
-      <c r="Q22" s="100"/>
-      <c r="R22" s="101"/>
-      <c r="S22" s="101"/>
-      <c r="T22" s="101"/>
-      <c r="U22" s="102"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="27"/>
       <c r="V22" s="18"/>
       <c r="W22" s="9"/>
-      <c r="X22" s="43"/>
-      <c r="Y22" s="43"/>
-      <c r="Z22" s="43"/>
-      <c r="AA22" s="43"/>
-      <c r="AB22" s="44"/>
+      <c r="X22" s="51"/>
+      <c r="Y22" s="51"/>
+      <c r="Z22" s="51"/>
+      <c r="AA22" s="51"/>
+      <c r="AB22" s="52"/>
     </row>
     <row r="23" spans="2:28" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="27"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="30"/>
       <c r="O23" s="16"/>
       <c r="P23" s="9"/>
-      <c r="Q23" s="100"/>
-      <c r="R23" s="101"/>
-      <c r="S23" s="101"/>
-      <c r="T23" s="101"/>
-      <c r="U23" s="102"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="27"/>
       <c r="V23" s="18"/>
       <c r="W23" s="9"/>
-      <c r="X23" s="43"/>
-      <c r="Y23" s="43"/>
-      <c r="Z23" s="43"/>
-      <c r="AA23" s="43"/>
-      <c r="AB23" s="44"/>
+      <c r="X23" s="51"/>
+      <c r="Y23" s="51"/>
+      <c r="Z23" s="51"/>
+      <c r="AA23" s="51"/>
+      <c r="AB23" s="52"/>
     </row>
     <row r="24" spans="2:28" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="25" t="s">
+      <c r="C24" s="32"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="27"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="30"/>
       <c r="O24" s="16"/>
       <c r="P24" s="9"/>
-      <c r="Q24" s="100"/>
-      <c r="R24" s="101"/>
-      <c r="S24" s="101"/>
-      <c r="T24" s="101"/>
-      <c r="U24" s="102"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="27"/>
       <c r="V24" s="18"/>
       <c r="W24" s="9"/>
-      <c r="X24" s="43"/>
-      <c r="Y24" s="43"/>
-      <c r="Z24" s="43"/>
-      <c r="AA24" s="43"/>
-      <c r="AB24" s="44"/>
+      <c r="X24" s="51"/>
+      <c r="Y24" s="51"/>
+      <c r="Z24" s="51"/>
+      <c r="AA24" s="51"/>
+      <c r="AB24" s="52"/>
     </row>
     <row r="25" spans="2:28" s="8" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="103" t="s">
+      <c r="B25" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="104"/>
-      <c r="D25" s="105"/>
-      <c r="E25" s="106" t="s">
+      <c r="C25" s="54"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="107"/>
-      <c r="G25" s="107"/>
-      <c r="H25" s="107"/>
-      <c r="I25" s="107"/>
-      <c r="J25" s="107"/>
-      <c r="K25" s="107"/>
-      <c r="L25" s="107"/>
-      <c r="M25" s="107"/>
-      <c r="N25" s="108"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="58"/>
       <c r="O25" s="19"/>
       <c r="P25" s="11"/>
-      <c r="Q25" s="109"/>
-      <c r="R25" s="110"/>
-      <c r="S25" s="110"/>
-      <c r="T25" s="110"/>
-      <c r="U25" s="111"/>
+      <c r="Q25" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="R25" s="60"/>
+      <c r="S25" s="60"/>
+      <c r="T25" s="60"/>
+      <c r="U25" s="61"/>
       <c r="V25" s="20"/>
       <c r="W25" s="11"/>
-      <c r="X25" s="112"/>
-      <c r="Y25" s="112"/>
-      <c r="Z25" s="112"/>
-      <c r="AA25" s="112"/>
-      <c r="AB25" s="113"/>
+      <c r="X25" s="62"/>
+      <c r="Y25" s="62"/>
+      <c r="Z25" s="62"/>
+      <c r="AA25" s="62"/>
+      <c r="AB25" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="E19:N19"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:AB14"/>
+    <mergeCell ref="B13:AB13"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:AB15"/>
+    <mergeCell ref="X18:AB18"/>
+    <mergeCell ref="X17:AB17"/>
+    <mergeCell ref="E18:N18"/>
+    <mergeCell ref="B16:D17"/>
+    <mergeCell ref="E16:N17"/>
+    <mergeCell ref="O16:U16"/>
+    <mergeCell ref="V16:AB16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="X2:AB5"/>
+    <mergeCell ref="I2:W3"/>
+    <mergeCell ref="B9:AB9"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="W7:Y7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="I4:W5"/>
+    <mergeCell ref="B2:H5"/>
+    <mergeCell ref="E21:N21"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="Q21:U21"/>
+    <mergeCell ref="X21:AB21"/>
+    <mergeCell ref="Q22:U22"/>
+    <mergeCell ref="X22:AB22"/>
+    <mergeCell ref="Q23:U23"/>
+    <mergeCell ref="X23:AB23"/>
+    <mergeCell ref="E22:N22"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:N23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:N25"/>
+    <mergeCell ref="Q25:U25"/>
+    <mergeCell ref="X25:AB25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:N24"/>
+    <mergeCell ref="Q24:U24"/>
+    <mergeCell ref="X24:AB24"/>
     <mergeCell ref="X20:AB20"/>
     <mergeCell ref="Q20:U20"/>
     <mergeCell ref="E20:N20"/>
@@ -4492,52 +4565,7 @@
     <mergeCell ref="U11:Y11"/>
     <mergeCell ref="Q19:U19"/>
     <mergeCell ref="X19:AB19"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:N25"/>
-    <mergeCell ref="Q25:U25"/>
-    <mergeCell ref="X25:AB25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:N24"/>
-    <mergeCell ref="Q24:U24"/>
-    <mergeCell ref="X24:AB24"/>
-    <mergeCell ref="X22:AB22"/>
-    <mergeCell ref="Q23:U23"/>
-    <mergeCell ref="X23:AB23"/>
-    <mergeCell ref="E22:N22"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:N23"/>
-    <mergeCell ref="E21:N21"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="Q21:U21"/>
-    <mergeCell ref="X21:AB21"/>
-    <mergeCell ref="Q22:U22"/>
-    <mergeCell ref="X2:AB5"/>
-    <mergeCell ref="I2:W3"/>
-    <mergeCell ref="B9:AB9"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="W7:Y7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="I4:W5"/>
-    <mergeCell ref="B2:H5"/>
     <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:N19"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:AB14"/>
-    <mergeCell ref="B13:AB13"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:AB15"/>
-    <mergeCell ref="X18:AB18"/>
-    <mergeCell ref="X17:AB17"/>
-    <mergeCell ref="E18:N18"/>
-    <mergeCell ref="B16:D17"/>
-    <mergeCell ref="E16:N17"/>
-    <mergeCell ref="O16:U16"/>
-    <mergeCell ref="V16:AB16"/>
-    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>